<commit_message>
Finished Simulated Annealing + Tabu Search
</commit_message>
<xml_diff>
--- a/Demand Forecast.xlsx
+++ b/Demand Forecast.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bff73b0ba30a6b9/Dokumen/College Files/OR/OR8/OR8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="11_64D8AB161DC56D41C99E36C615E87276769E86C4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12CDCD87-09EB-4CDA-9D05-36423E43656B}"/>
+  <xr:revisionPtr revIDLastSave="252" documentId="11_64D8AB161DC56D41C99E36C615E87276769E86C4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{667D327D-7D28-4087-B0BD-0166108FF829}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forecast" sheetId="1" r:id="rId1"/>
     <sheet name="ProductDataperState" sheetId="2" r:id="rId2"/>
     <sheet name="Product Data" sheetId="5" r:id="rId3"/>
     <sheet name="ProductWeigh" sheetId="3" r:id="rId4"/>
-    <sheet name="Handling Out Costs" sheetId="4" r:id="rId5"/>
-    <sheet name="__AIMMS_SETUP__" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
+    <sheet name="Handling Out Costs" sheetId="4" r:id="rId6"/>
+    <sheet name="__AIMMS_SETUP__" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast!$A$1:$A$53</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="95">
   <si>
     <t>Initialization</t>
   </si>
@@ -317,6 +318,15 @@
   </si>
   <si>
     <t>boxes in pallet</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Small shipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$7 </t>
   </si>
 </sst>
 </file>
@@ -1020,8 +1030,8 @@
   </sheetPr>
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1104,13 +1114,13 @@
       </c>
       <c r="H2" s="51">
         <f>SUM(ProductWeigh!B2:F2)</f>
-        <v>21725.913800000002</v>
+        <v>23788.0802</v>
       </c>
       <c r="I2" s="50">
         <v>52</v>
       </c>
       <c r="J2" s="58">
-        <f>ROUND(0.2*I2,0)</f>
+        <f>_xlfn.FLOOR.MATH(I2/5,1)</f>
         <v>10</v>
       </c>
       <c r="K2" s="62">
@@ -1123,7 +1133,7 @@
       </c>
       <c r="M2" s="62">
         <f>H2-L2</f>
-        <v>21460.913800000002</v>
+        <v>23523.0802</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1150,13 +1160,13 @@
       </c>
       <c r="H3" s="51">
         <f>SUM(ProductWeigh!B3:F3)</f>
-        <v>151909.1047</v>
+        <v>165656.88069999998</v>
       </c>
       <c r="I3" s="50">
         <v>301</v>
       </c>
       <c r="J3" s="58">
-        <f t="shared" ref="J3:J52" si="0">ROUND(0.2*I3,0)</f>
+        <f t="shared" ref="J3:J52" si="0">_xlfn.FLOOR.MATH(I3/5,1)</f>
         <v>60</v>
       </c>
       <c r="K3" s="62">
@@ -1169,7 +1179,7 @@
       </c>
       <c r="M3" s="62">
         <f t="shared" ref="M3:M52" si="3">H3-L3</f>
-        <v>150319.1047</v>
+        <v>164066.88069999998</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1196,7 +1206,7 @@
       </c>
       <c r="H4" s="51">
         <f>SUM(ProductWeigh!B4:F4)</f>
-        <v>91232.880600000004</v>
+        <v>99481.546200000012</v>
       </c>
       <c r="I4" s="50">
         <v>172</v>
@@ -1215,7 +1225,7 @@
       </c>
       <c r="M4" s="62">
         <f t="shared" si="3"/>
-        <v>90331.880600000004</v>
+        <v>98580.546200000012</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1242,26 +1252,26 @@
       </c>
       <c r="H5" s="51">
         <f>SUM(ProductWeigh!B5:F5)</f>
-        <v>220708.1409</v>
+        <v>240986.11049999998</v>
       </c>
       <c r="I5" s="50">
         <v>428</v>
       </c>
       <c r="J5" s="58">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K5" s="62">
         <f t="shared" si="1"/>
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L5" s="61">
         <f t="shared" si="2"/>
-        <v>2279</v>
+        <v>2252.5</v>
       </c>
       <c r="M5" s="62">
         <f t="shared" si="3"/>
-        <v>218429.1409</v>
+        <v>238733.61049999998</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1288,7 +1298,7 @@
       </c>
       <c r="H6" s="51">
         <f>SUM(ProductWeigh!B6:F6)</f>
-        <v>1158740.0586999999</v>
+        <v>1263566.8507000001</v>
       </c>
       <c r="I6" s="50">
         <v>2176</v>
@@ -1307,7 +1317,7 @@
       </c>
       <c r="M6" s="62">
         <f t="shared" si="3"/>
-        <v>1147212.5586999999</v>
+        <v>1252039.3507000001</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1334,7 +1344,7 @@
       </c>
       <c r="H7" s="51">
         <f>SUM(ProductWeigh!B7:F7)</f>
-        <v>174791.6159</v>
+        <v>190601.5583</v>
       </c>
       <c r="I7" s="50">
         <v>520</v>
@@ -1353,7 +1363,7 @@
       </c>
       <c r="M7" s="62">
         <f t="shared" si="3"/>
-        <v>172035.6159</v>
+        <v>187845.5583</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1380,7 +1390,7 @@
       </c>
       <c r="H8" s="51">
         <f>SUM(ProductWeigh!B8:F8)</f>
-        <v>107330.935</v>
+        <v>117298.0726</v>
       </c>
       <c r="I8" s="50">
         <v>266</v>
@@ -1399,7 +1409,7 @@
       </c>
       <c r="M8" s="62">
         <f t="shared" si="3"/>
-        <v>105926.435</v>
+        <v>115893.5726</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1426,7 +1436,7 @@
       </c>
       <c r="H9" s="51">
         <f>SUM(ProductWeigh!B9:F9)</f>
-        <v>19959.803</v>
+        <v>22021.969400000002</v>
       </c>
       <c r="I9" s="50">
         <v>55</v>
@@ -1445,7 +1455,7 @@
       </c>
       <c r="M9" s="62">
         <f t="shared" si="3"/>
-        <v>19668.303</v>
+        <v>21730.469400000002</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1472,7 +1482,7 @@
       </c>
       <c r="H10" s="51">
         <f>SUM(ProductWeigh!B10:F10)</f>
-        <v>30366.241999999998</v>
+        <v>33459.491600000001</v>
       </c>
       <c r="I10" s="50">
         <v>72</v>
@@ -1491,7 +1501,7 @@
       </c>
       <c r="M10" s="62">
         <f t="shared" si="3"/>
-        <v>29995.241999999998</v>
+        <v>33088.491600000001</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1518,7 +1528,7 @@
       </c>
       <c r="H11" s="51">
         <f>SUM(ProductWeigh!B11:F11)</f>
-        <v>672392.77709999995</v>
+        <v>733226.68589999992</v>
       </c>
       <c r="I11" s="50">
         <v>1422</v>
@@ -1537,7 +1547,7 @@
       </c>
       <c r="M11" s="62">
         <f t="shared" si="3"/>
-        <v>664866.77709999995</v>
+        <v>725700.68589999992</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1564,7 +1574,7 @@
       </c>
       <c r="H12" s="51">
         <f>SUM(ProductWeigh!B12:F12)</f>
-        <v>327755.85840000003</v>
+        <v>357657.27120000002</v>
       </c>
       <c r="I12" s="50">
         <v>722</v>
@@ -1583,7 +1593,7 @@
       </c>
       <c r="M12" s="62">
         <f t="shared" si="3"/>
-        <v>323939.85840000003</v>
+        <v>353841.27120000002</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1610,7 +1620,7 @@
       </c>
       <c r="H13" s="51">
         <f>SUM(ProductWeigh!B13:F13)</f>
-        <v>42417.615099999995</v>
+        <v>46541.947899999999</v>
       </c>
       <c r="I13" s="50">
         <v>102</v>
@@ -1629,7 +1639,7 @@
       </c>
       <c r="M13" s="62">
         <f t="shared" si="3"/>
-        <v>41887.615099999995</v>
+        <v>46011.947899999999</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1656,7 +1666,7 @@
       </c>
       <c r="H14" s="51">
         <f>SUM(ProductWeigh!B14:F14)</f>
-        <v>95063.782199999987</v>
+        <v>103999.8366</v>
       </c>
       <c r="I14" s="50">
         <v>211</v>
@@ -1675,7 +1685,7 @@
       </c>
       <c r="M14" s="62">
         <f t="shared" si="3"/>
-        <v>93950.782199999987</v>
+        <v>102886.8366</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1702,26 +1712,26 @@
       </c>
       <c r="H15" s="51">
         <f>SUM(ProductWeigh!B15:F15)</f>
-        <v>58215.772199999999</v>
+        <v>63714.882599999997</v>
       </c>
       <c r="I15" s="50">
         <v>123</v>
       </c>
       <c r="J15" s="58">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" s="62">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L15" s="61">
         <f t="shared" si="2"/>
-        <v>662.5</v>
+        <v>636</v>
       </c>
       <c r="M15" s="62">
         <f t="shared" si="3"/>
-        <v>57553.272199999999</v>
+        <v>63078.882599999997</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1748,26 +1758,26 @@
       </c>
       <c r="H16" s="51">
         <f>SUM(ProductWeigh!B16:F16)</f>
-        <v>372936.1777</v>
+        <v>406961.92330000002</v>
       </c>
       <c r="I16" s="50">
         <v>813</v>
       </c>
       <c r="J16" s="58">
         <f t="shared" si="0"/>
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K16" s="62">
         <f t="shared" si="1"/>
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="L16" s="61">
         <f t="shared" si="2"/>
-        <v>4319.5</v>
+        <v>4293</v>
       </c>
       <c r="M16" s="62">
         <f t="shared" si="3"/>
-        <v>368616.6777</v>
+        <v>402668.92330000002</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1794,7 +1804,7 @@
       </c>
       <c r="H17" s="51">
         <f>SUM(ProductWeigh!B17:F17)</f>
-        <v>203966.50349999999</v>
+        <v>222526.00109999999</v>
       </c>
       <c r="I17" s="50">
         <v>387</v>
@@ -1813,7 +1823,7 @@
       </c>
       <c r="M17" s="62">
         <f t="shared" si="3"/>
-        <v>201926.00349999999</v>
+        <v>220485.50109999999</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1840,7 +1850,7 @@
       </c>
       <c r="H18" s="51">
         <f>SUM(ProductWeigh!B18:F18)</f>
-        <v>87451.956399999995</v>
+        <v>95356.927599999995</v>
       </c>
       <c r="I18" s="50">
         <v>216</v>
@@ -1859,7 +1869,7 @@
       </c>
       <c r="M18" s="62">
         <f t="shared" si="3"/>
-        <v>86312.456399999995</v>
+        <v>94217.427599999995</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1886,7 +1896,7 @@
       </c>
       <c r="H19" s="51">
         <f>SUM(ProductWeigh!B19:F19)</f>
-        <v>134401.67969999998</v>
+        <v>146774.67809999999</v>
       </c>
       <c r="I19" s="50">
         <v>241</v>
@@ -1905,7 +1915,7 @@
       </c>
       <c r="M19" s="62">
         <f t="shared" si="3"/>
-        <v>133129.67969999998</v>
+        <v>145502.67809999999</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1932,26 +1942,26 @@
       </c>
       <c r="H20" s="51">
         <f>SUM(ProductWeigh!B20:F20)</f>
-        <v>135946.87839999999</v>
+        <v>148319.8768</v>
       </c>
       <c r="I20" s="50">
         <v>269</v>
       </c>
       <c r="J20" s="58">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K20" s="62">
         <f t="shared" si="1"/>
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L20" s="61">
         <f t="shared" si="2"/>
-        <v>1431</v>
+        <v>1404.5</v>
       </c>
       <c r="M20" s="62">
         <f t="shared" si="3"/>
-        <v>134515.87839999999</v>
+        <v>146915.3768</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1978,26 +1988,26 @@
       </c>
       <c r="H21" s="51">
         <f>SUM(ProductWeigh!B21:F21)</f>
-        <v>208139.07130000001</v>
+        <v>227042.26329999999</v>
       </c>
       <c r="I21" s="50">
         <v>498</v>
       </c>
       <c r="J21" s="58">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K21" s="62">
         <f t="shared" si="1"/>
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="L21" s="61">
         <f t="shared" si="2"/>
-        <v>2650</v>
+        <v>2623.5</v>
       </c>
       <c r="M21" s="62">
         <f t="shared" si="3"/>
-        <v>205489.07130000001</v>
+        <v>224418.76329999999</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2024,7 +2034,7 @@
       </c>
       <c r="H22" s="51">
         <f>SUM(ProductWeigh!B22:F22)</f>
-        <v>183571.64840000001</v>
+        <v>200412.674</v>
       </c>
       <c r="I22" s="50">
         <v>477</v>
@@ -2043,7 +2053,7 @@
       </c>
       <c r="M22" s="62">
         <f t="shared" si="3"/>
-        <v>181054.14840000001</v>
+        <v>197895.174</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2070,7 +2080,7 @@
       </c>
       <c r="H23" s="51">
         <f>SUM(ProductWeigh!B23:F23)</f>
-        <v>41482.256500000003</v>
+        <v>45262.894899999999</v>
       </c>
       <c r="I23" s="50">
         <v>87</v>
@@ -2089,7 +2099,7 @@
       </c>
       <c r="M23" s="62">
         <f t="shared" si="3"/>
-        <v>41031.756500000003</v>
+        <v>44812.394899999999</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2116,7 +2126,7 @@
       </c>
       <c r="H24" s="51">
         <f>SUM(ProductWeigh!B24:F24)</f>
-        <v>298331.44309999997</v>
+        <v>325483.30070000002</v>
       </c>
       <c r="I24" s="50">
         <v>672</v>
@@ -2135,7 +2145,7 @@
       </c>
       <c r="M24" s="62">
         <f t="shared" si="3"/>
-        <v>294780.44309999997</v>
+        <v>321932.30070000002</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2162,7 +2172,7 @@
       </c>
       <c r="H25" s="51">
         <f>SUM(ProductWeigh!B25:F25)</f>
-        <v>170604.84179999999</v>
+        <v>186071.08980000002</v>
       </c>
       <c r="I25" s="50">
         <v>602</v>
@@ -2181,7 +2191,7 @@
       </c>
       <c r="M25" s="62">
         <f t="shared" si="3"/>
-        <v>167424.84179999999</v>
+        <v>182891.08980000002</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2208,7 +2218,7 @@
       </c>
       <c r="H26" s="51">
         <f>SUM(ProductWeigh!B26:F26)</f>
-        <v>184094.4381</v>
+        <v>200935.46369999999</v>
       </c>
       <c r="I26" s="50">
         <v>536</v>
@@ -2227,7 +2237,7 @@
       </c>
       <c r="M26" s="62">
         <f t="shared" si="3"/>
-        <v>181258.9381</v>
+        <v>198099.96369999999</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2254,26 +2264,26 @@
       </c>
       <c r="H27" s="51">
         <f>SUM(ProductWeigh!B27:F27)</f>
-        <v>87425.563200000004</v>
+        <v>95330.534400000004</v>
       </c>
       <c r="I27" s="50">
         <v>274</v>
       </c>
       <c r="J27" s="58">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K27" s="62">
         <f t="shared" si="1"/>
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L27" s="61">
         <f t="shared" si="2"/>
-        <v>1457.5</v>
+        <v>1431</v>
       </c>
       <c r="M27" s="62">
         <f t="shared" si="3"/>
-        <v>85968.063200000004</v>
+        <v>93899.534400000004</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2300,26 +2310,26 @@
       </c>
       <c r="H28" s="51">
         <f>SUM(ProductWeigh!B28:F28)</f>
-        <v>184099.47</v>
+        <v>187192.71959999998</v>
       </c>
       <c r="I28" s="50">
         <v>83</v>
       </c>
       <c r="J28" s="58">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K28" s="62">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L28" s="61">
         <f t="shared" si="2"/>
-        <v>450.5</v>
+        <v>424</v>
       </c>
       <c r="M28" s="62">
         <f t="shared" si="3"/>
-        <v>183648.97</v>
+        <v>186768.71959999998</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2346,26 +2356,26 @@
       </c>
       <c r="H29" s="51">
         <f>SUM(ProductWeigh!B29:F29)</f>
-        <v>322159.86009999999</v>
+        <v>351373.88410000002</v>
       </c>
       <c r="I29" s="50">
         <v>878</v>
       </c>
       <c r="J29" s="58">
         <f t="shared" si="0"/>
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K29" s="62">
         <f t="shared" si="1"/>
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="L29" s="61">
         <f t="shared" si="2"/>
-        <v>4664</v>
+        <v>4637.5</v>
       </c>
       <c r="M29" s="62">
         <f t="shared" si="3"/>
-        <v>317495.86009999999</v>
+        <v>346736.38410000002</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2392,26 +2402,26 @@
       </c>
       <c r="H30" s="51">
         <f>SUM(ProductWeigh!B30:F30)</f>
-        <v>23011.677</v>
+        <v>25417.537799999998</v>
       </c>
       <c r="I30" s="50">
         <v>68</v>
       </c>
       <c r="J30" s="58">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K30" s="62">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L30" s="61">
         <f t="shared" si="2"/>
-        <v>371</v>
+        <v>344.5</v>
       </c>
       <c r="M30" s="62">
         <f t="shared" si="3"/>
-        <v>22640.677</v>
+        <v>25073.037799999998</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2438,26 +2448,26 @@
       </c>
       <c r="H31" s="51">
         <f>SUM(ProductWeigh!B31:F31)</f>
-        <v>58659.188099999999</v>
+        <v>64158.298499999997</v>
       </c>
       <c r="I31" s="50">
         <v>133</v>
       </c>
       <c r="J31" s="58">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K31" s="62">
         <f t="shared" si="1"/>
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L31" s="61">
         <f t="shared" si="2"/>
-        <v>715.5</v>
+        <v>689</v>
       </c>
       <c r="M31" s="62">
         <f t="shared" si="3"/>
-        <v>57943.688099999999</v>
+        <v>63469.298499999997</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2484,26 +2494,26 @@
       </c>
       <c r="H32" s="51">
         <f>SUM(ProductWeigh!B32:F32)</f>
-        <v>41689.531100000007</v>
+        <v>45470.169500000004</v>
       </c>
       <c r="I32" s="50">
         <v>123</v>
       </c>
       <c r="J32" s="58">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K32" s="62">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L32" s="61">
         <f t="shared" si="2"/>
-        <v>662.5</v>
+        <v>636</v>
       </c>
       <c r="M32" s="62">
         <f t="shared" si="3"/>
-        <v>41027.031100000007</v>
+        <v>44834.169500000004</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2530,26 +2540,26 @@
       </c>
       <c r="H33" s="51">
         <f>SUM(ProductWeigh!B33:F33)</f>
-        <v>276194.2254</v>
+        <v>301283.9166</v>
       </c>
       <c r="I33" s="50">
         <v>823</v>
       </c>
       <c r="J33" s="58">
         <f t="shared" si="0"/>
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K33" s="62">
         <f t="shared" si="1"/>
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="L33" s="61">
         <f t="shared" si="2"/>
-        <v>4372.5</v>
+        <v>4346</v>
       </c>
       <c r="M33" s="62">
         <f t="shared" si="3"/>
-        <v>271821.7254</v>
+        <v>296937.9166</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2576,7 +2586,7 @@
       </c>
       <c r="H34" s="51">
         <f>SUM(ProductWeigh!B34:F34)</f>
-        <v>62723.515400000004</v>
+        <v>68566.320200000002</v>
       </c>
       <c r="I34" s="50">
         <v>121</v>
@@ -2595,7 +2605,7 @@
       </c>
       <c r="M34" s="62">
         <f t="shared" si="3"/>
-        <v>62087.515400000004</v>
+        <v>67930.320200000002</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2622,26 +2632,26 @@
       </c>
       <c r="H35" s="51">
         <f>SUM(ProductWeigh!B35:F35)</f>
-        <v>94983.152199999997</v>
+        <v>103575.5122</v>
       </c>
       <c r="I35" s="50">
         <v>223</v>
       </c>
       <c r="J35" s="58">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K35" s="62">
         <f t="shared" si="1"/>
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="L35" s="61">
         <f t="shared" si="2"/>
-        <v>1192.5</v>
+        <v>1166</v>
       </c>
       <c r="M35" s="62">
         <f t="shared" si="3"/>
-        <v>93790.652199999997</v>
+        <v>102409.5122</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2668,26 +2678,26 @@
       </c>
       <c r="H36" s="51">
         <f>SUM(ProductWeigh!B36:F36)</f>
-        <v>582071.66209999996</v>
+        <v>634656.90529999998</v>
       </c>
       <c r="I36" s="50">
         <v>1344</v>
       </c>
       <c r="J36" s="58">
         <f t="shared" si="0"/>
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K36" s="62">
         <f t="shared" si="1"/>
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="L36" s="61">
         <f t="shared" si="2"/>
-        <v>7128.5</v>
+        <v>7102</v>
       </c>
       <c r="M36" s="62">
         <f t="shared" si="3"/>
-        <v>574943.16209999996</v>
+        <v>627554.90529999998</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2714,7 +2724,7 @@
       </c>
       <c r="H37" s="51">
         <f>SUM(ProductWeigh!B37:F37)</f>
-        <v>350229.47729999997</v>
+        <v>382193.05649999995</v>
       </c>
       <c r="I37" s="50">
         <v>887</v>
@@ -2733,7 +2743,7 @@
       </c>
       <c r="M37" s="62">
         <f t="shared" si="3"/>
-        <v>345538.97729999997</v>
+        <v>377502.55649999995</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2760,26 +2770,26 @@
       </c>
       <c r="H38" s="51">
         <f>SUM(ProductWeigh!B38:F38)</f>
-        <v>120456.48939999999</v>
+        <v>131454.7102</v>
       </c>
       <c r="I38" s="50">
         <v>299</v>
       </c>
       <c r="J38" s="58">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K38" s="62">
         <f t="shared" si="1"/>
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L38" s="61">
         <f t="shared" si="2"/>
-        <v>1590</v>
+        <v>1563.5</v>
       </c>
       <c r="M38" s="62">
         <f t="shared" si="3"/>
-        <v>118866.48939999999</v>
+        <v>129891.2102</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2806,7 +2816,7 @@
       </c>
       <c r="H39" s="51">
         <f>SUM(ProductWeigh!B39:F39)</f>
-        <v>125595.87079999999</v>
+        <v>137281.4804</v>
       </c>
       <c r="I39" s="50">
         <v>410</v>
@@ -2825,7 +2835,7 @@
       </c>
       <c r="M39" s="62">
         <f t="shared" si="3"/>
-        <v>123422.87079999999</v>
+        <v>135108.4804</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2852,26 +2862,26 @@
       </c>
       <c r="H40" s="51">
         <f>SUM(ProductWeigh!B40:F40)</f>
-        <v>385264.86920000002</v>
+        <v>420321.69799999997</v>
       </c>
       <c r="I40" s="50">
         <v>758</v>
       </c>
       <c r="J40" s="58">
         <f t="shared" si="0"/>
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K40" s="62">
         <f t="shared" si="1"/>
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="L40" s="61">
         <f t="shared" si="2"/>
-        <v>4028</v>
+        <v>4001.5</v>
       </c>
       <c r="M40" s="62">
         <f t="shared" si="3"/>
-        <v>381236.86920000002</v>
+        <v>416320.19799999997</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2898,7 +2908,7 @@
       </c>
       <c r="H41" s="51">
         <f>SUM(ProductWeigh!B41:F41)</f>
-        <v>32447.859100000001</v>
+        <v>35541.108699999997</v>
       </c>
       <c r="I41" s="50">
         <v>70</v>
@@ -2917,7 +2927,7 @@
       </c>
       <c r="M41" s="62">
         <f t="shared" si="3"/>
-        <v>32076.859100000001</v>
+        <v>35170.108699999997</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2944,7 +2954,7 @@
       </c>
       <c r="H42" s="51">
         <f>SUM(ProductWeigh!B42:F42)</f>
-        <v>159824.0166</v>
+        <v>174259.1814</v>
       </c>
       <c r="I42" s="50">
         <v>315</v>
@@ -2963,7 +2973,7 @@
       </c>
       <c r="M42" s="62">
         <f t="shared" si="3"/>
-        <v>158154.5166</v>
+        <v>172589.6814</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2990,7 +3000,7 @@
       </c>
       <c r="H43" s="51">
         <f>SUM(ProductWeigh!B43:F43)</f>
-        <v>27067.499199999998</v>
+        <v>29817.054400000001</v>
       </c>
       <c r="I43" s="50">
         <v>66</v>
@@ -3009,7 +3019,7 @@
       </c>
       <c r="M43" s="62">
         <f t="shared" si="3"/>
-        <v>26722.999199999998</v>
+        <v>29472.554400000001</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3036,7 +3046,7 @@
       </c>
       <c r="H44" s="51">
         <f>SUM(ProductWeigh!B44:F44)</f>
-        <v>211848.7346</v>
+        <v>231095.62099999998</v>
       </c>
       <c r="I44" s="50">
         <v>712</v>
@@ -3055,7 +3065,7 @@
       </c>
       <c r="M44" s="62">
         <f t="shared" si="3"/>
-        <v>208085.7346</v>
+        <v>227332.62099999998</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3082,7 +3092,7 @@
       </c>
       <c r="H45" s="51">
         <f>SUM(ProductWeigh!B45:F45)</f>
-        <v>907017.24179999996</v>
+        <v>989160.2034</v>
       </c>
       <c r="I45" s="50">
         <v>2221</v>
@@ -3101,7 +3111,7 @@
       </c>
       <c r="M45" s="62">
         <f t="shared" si="3"/>
-        <v>895251.24179999996</v>
+        <v>977394.2034</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3128,26 +3138,26 @@
       </c>
       <c r="H46" s="51">
         <f>SUM(ProductWeigh!B46:F46)</f>
-        <v>101548.976</v>
+        <v>110828.7248</v>
       </c>
       <c r="I46" s="50">
         <v>278</v>
       </c>
       <c r="J46" s="58">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K46" s="62">
         <f t="shared" si="1"/>
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L46" s="61">
         <f t="shared" si="2"/>
-        <v>1484</v>
+        <v>1457.5</v>
       </c>
       <c r="M46" s="62">
         <f t="shared" si="3"/>
-        <v>100064.976</v>
+        <v>109371.2248</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3174,26 +3184,26 @@
       </c>
       <c r="H47" s="51">
         <f>SUM(ProductWeigh!B47:F47)</f>
-        <v>258918.43119999999</v>
+        <v>282633.34480000002</v>
       </c>
       <c r="I47" s="50">
         <v>513</v>
       </c>
       <c r="J47" s="58">
         <f t="shared" si="0"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K47" s="62">
         <f t="shared" si="1"/>
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="L47" s="61">
         <f t="shared" si="2"/>
-        <v>2729.5</v>
+        <v>2703</v>
       </c>
       <c r="M47" s="62">
         <f t="shared" si="3"/>
-        <v>256188.93119999999</v>
+        <v>279930.34480000002</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3220,7 +3230,7 @@
       </c>
       <c r="H48" s="51">
         <f>SUM(ProductWeigh!B48:F48)</f>
-        <v>18933.712200000002</v>
+        <v>20995.878599999996</v>
       </c>
       <c r="I48" s="50">
         <v>66</v>
@@ -3239,7 +3249,7 @@
       </c>
       <c r="M48" s="62">
         <f t="shared" si="3"/>
-        <v>18589.212200000002</v>
+        <v>20651.378599999996</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3266,7 +3276,7 @@
       </c>
       <c r="H49" s="51">
         <f>SUM(ProductWeigh!B49:F49)</f>
-        <v>232046.27059999999</v>
+        <v>253355.32339999999</v>
       </c>
       <c r="I49" s="50">
         <v>521</v>
@@ -3285,7 +3295,7 @@
       </c>
       <c r="M49" s="62">
         <f t="shared" si="3"/>
-        <v>229290.27059999999</v>
+        <v>250599.32339999999</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3312,7 +3322,7 @@
       </c>
       <c r="H50" s="51">
         <f>SUM(ProductWeigh!B50:F50)</f>
-        <v>175528.8357</v>
+        <v>191682.4725</v>
       </c>
       <c r="I50" s="50">
         <v>387</v>
@@ -3331,7 +3341,7 @@
       </c>
       <c r="M50" s="62">
         <f t="shared" si="3"/>
-        <v>173488.3357</v>
+        <v>189641.9725</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3358,7 +3368,7 @@
       </c>
       <c r="H51" s="51">
         <f>SUM(ProductWeigh!B51:F51)</f>
-        <v>52585.064899999998</v>
+        <v>57396.786500000002</v>
       </c>
       <c r="I51" s="50">
         <v>142</v>
@@ -3377,7 +3387,7 @@
       </c>
       <c r="M51" s="62">
         <f t="shared" si="3"/>
-        <v>51843.064899999998</v>
+        <v>56654.786500000002</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3404,7 +3414,7 @@
       </c>
       <c r="H52" s="51">
         <f>SUM(ProductWeigh!B52:F52)</f>
-        <v>17217.5399</v>
+        <v>18936.011899999998</v>
       </c>
       <c r="I52" s="50">
         <v>46</v>
@@ -3423,7 +3433,7 @@
       </c>
       <c r="M52" s="62">
         <f t="shared" si="3"/>
-        <v>16979.0399</v>
+        <v>18697.511899999998</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3436,6 +3446,10 @@
       <c r="H53" s="41"/>
       <c r="I53" s="35"/>
       <c r="J53" s="38"/>
+      <c r="L53" s="37">
+        <f>SUM(L2:L52)*7</f>
+        <v>856268</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:A53" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -3450,7 +3464,7 @@
   </sheetPr>
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -6656,7 +6670,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6764,7 +6778,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6803,8 +6817,8 @@
         <v>40</v>
       </c>
       <c r="B2" s="8">
-        <f>ProductDataperState!G2*'Product Data'!C$2</f>
-        <v>555.43469999999991</v>
+        <f>Forecast!B2*'Product Data'!C$2</f>
+        <v>2617.6010999999999</v>
       </c>
       <c r="C2" s="8">
         <f>Forecast!C2*'Product Data'!$C$3</f>
@@ -6829,8 +6843,8 @@
         <v>41</v>
       </c>
       <c r="B3" s="8">
-        <f>ProductDataperState!G3*'Product Data'!C$2</f>
-        <v>4481.3248999999996</v>
+        <f>Forecast!B3*'Product Data'!C$2</f>
+        <v>18229.100899999998</v>
       </c>
       <c r="C3" s="8">
         <f>Forecast!C3*'Product Data'!$C$3</f>
@@ -6854,8 +6868,8 @@
         <v>42</v>
       </c>
       <c r="B4" s="8">
-        <f>ProductDataperState!G4*'Product Data'!C$2</f>
-        <v>2698.4101999999998</v>
+        <f>Forecast!B4*'Product Data'!C$2</f>
+        <v>10947.075799999999</v>
       </c>
       <c r="C4" s="8">
         <f>Forecast!C4*'Product Data'!$C$3</f>
@@ -6879,8 +6893,8 @@
         <v>43</v>
       </c>
       <c r="B5" s="8">
-        <f>ProductDataperState!G5*'Product Data'!C$2</f>
-        <v>6240.7128999999995</v>
+        <f>Forecast!B5*'Product Data'!C$2</f>
+        <v>26518.682499999999</v>
       </c>
       <c r="C5" s="8">
         <f>Forecast!C5*'Product Data'!$C$3</f>
@@ -6904,8 +6918,8 @@
         <v>28</v>
       </c>
       <c r="B6" s="8">
-        <f>ProductDataperState!G6*'Product Data'!C$2</f>
-        <v>34218.050799999997</v>
+        <f>Forecast!B6*'Product Data'!C$2</f>
+        <v>139044.84279999998</v>
       </c>
       <c r="C6" s="8">
         <f>Forecast!C6*'Product Data'!$C$3</f>
@@ -6929,8 +6943,8 @@
         <v>44</v>
       </c>
       <c r="B7" s="8">
-        <f>ProductDataperState!G7*'Product Data'!C$2</f>
-        <v>5163.5991999999997</v>
+        <f>Forecast!B7*'Product Data'!C$2</f>
+        <v>20973.541599999997</v>
       </c>
       <c r="C7" s="8">
         <f>Forecast!C7*'Product Data'!$C$3</f>
@@ -6954,8 +6968,8 @@
         <v>45</v>
       </c>
       <c r="B8" s="8">
-        <f>ProductDataperState!G8*'Product Data'!C$2</f>
-        <v>2940.8374999999996</v>
+        <f>Forecast!B8*'Product Data'!C$2</f>
+        <v>12907.9751</v>
       </c>
       <c r="C8" s="8">
         <f>Forecast!C8*'Product Data'!$C$3</f>
@@ -6979,8 +6993,8 @@
         <v>46</v>
       </c>
       <c r="B9" s="8">
-        <f>ProductDataperState!G9*'Product Data'!C$2</f>
-        <v>361.08369999999996</v>
+        <f>Forecast!B9*'Product Data'!C$2</f>
+        <v>2423.2500999999997</v>
       </c>
       <c r="C9" s="8">
         <f>Forecast!C9*'Product Data'!$C$3</f>
@@ -7004,8 +7018,8 @@
         <v>47</v>
       </c>
       <c r="B10" s="8">
-        <f>ProductDataperState!G10*'Product Data'!C$2</f>
-        <v>589.19039999999995</v>
+        <f>Forecast!B10*'Product Data'!C$2</f>
+        <v>3682.4399999999996</v>
       </c>
       <c r="C10" s="8">
         <f>Forecast!C10*'Product Data'!$C$3</f>
@@ -7029,8 +7043,8 @@
         <v>48</v>
       </c>
       <c r="B11" s="8">
-        <f>ProductDataperState!G11*'Product Data'!C$2</f>
-        <v>19851.420299999998</v>
+        <f>Forecast!B11*'Product Data'!C$2</f>
+        <v>80685.329099999988</v>
       </c>
       <c r="C11" s="8">
         <f>Forecast!C11*'Product Data'!$C$3</f>
@@ -7054,8 +7068,8 @@
         <v>49</v>
       </c>
       <c r="B12" s="8">
-        <f>ProductDataperState!G12*'Product Data'!C$2</f>
-        <v>9455.6875999999993</v>
+        <f>Forecast!B12*'Product Data'!C$2</f>
+        <v>39357.100399999996</v>
       </c>
       <c r="C12" s="8">
         <f>Forecast!C12*'Product Data'!$C$3</f>
@@ -7079,8 +7093,8 @@
         <v>50</v>
       </c>
       <c r="B13" s="8">
-        <f>ProductDataperState!G13*'Product Data'!C$2</f>
-        <v>997.32749999999987</v>
+        <f>Forecast!B13*'Product Data'!C$2</f>
+        <v>5121.6602999999996</v>
       </c>
       <c r="C13" s="8">
         <f>Forecast!C13*'Product Data'!$C$3</f>
@@ -7104,8 +7118,8 @@
         <v>51</v>
       </c>
       <c r="B14" s="8">
-        <f>ProductDataperState!G14*'Product Data'!C$2</f>
-        <v>2508.1507999999999</v>
+        <f>Forecast!B14*'Product Data'!C$2</f>
+        <v>11444.205199999999</v>
       </c>
       <c r="C14" s="8">
         <f>Forecast!C14*'Product Data'!$C$3</f>
@@ -7129,8 +7143,8 @@
         <v>52</v>
       </c>
       <c r="B15" s="8">
-        <f>ProductDataperState!G15*'Product Data'!C$2</f>
-        <v>1511.8462</v>
+        <f>Forecast!B15*'Product Data'!C$2</f>
+        <v>7010.9565999999995</v>
       </c>
       <c r="C15" s="8">
         <f>Forecast!C15*'Product Data'!$C$3</f>
@@ -7155,8 +7169,8 @@
         <v>25</v>
       </c>
       <c r="B16" s="8">
-        <f>ProductDataperState!G16*'Product Data'!C$2</f>
-        <v>10756.8164</v>
+        <f>Forecast!B16*'Product Data'!C$2</f>
+        <v>44782.561999999998</v>
       </c>
       <c r="C16" s="8">
         <f>Forecast!C16*'Product Data'!$C$3</f>
@@ -7180,8 +7194,8 @@
         <v>53</v>
       </c>
       <c r="B17" s="8">
-        <f>ProductDataperState!G17*'Product Data'!C$2</f>
-        <v>5927.7054999999991</v>
+        <f>Forecast!B17*'Product Data'!C$2</f>
+        <v>24487.203099999999</v>
       </c>
       <c r="C17" s="8">
         <f>Forecast!C17*'Product Data'!$C$3</f>
@@ -7205,8 +7219,8 @@
         <v>27</v>
       </c>
       <c r="B18" s="8">
-        <f>ProductDataperState!G18*'Product Data'!C$2</f>
-        <v>2587.9369999999999</v>
+        <f>Forecast!B18*'Product Data'!C$2</f>
+        <v>10492.9082</v>
       </c>
       <c r="C18" s="8">
         <f>Forecast!C18*'Product Data'!$C$3</f>
@@ -7230,8 +7244,8 @@
         <v>54</v>
       </c>
       <c r="B19" s="8">
-        <f>ProductDataperState!G19*'Product Data'!C$2</f>
-        <v>3778.5925999999995</v>
+        <f>Forecast!B19*'Product Data'!C$2</f>
+        <v>16151.590999999999</v>
       </c>
       <c r="C19" s="8">
         <f>Forecast!C19*'Product Data'!$C$3</f>
@@ -7255,8 +7269,8 @@
         <v>55</v>
       </c>
       <c r="B20" s="8">
-        <f>ProductDataperState!G20*'Product Data'!C$2</f>
-        <v>3948.3939999999998</v>
+        <f>Forecast!B20*'Product Data'!C$2</f>
+        <v>16321.392399999999</v>
       </c>
       <c r="C20" s="8">
         <f>Forecast!C20*'Product Data'!$C$3</f>
@@ -7280,8 +7294,8 @@
         <v>56</v>
       </c>
       <c r="B21" s="8">
-        <f>ProductDataperState!G21*'Product Data'!C$2</f>
-        <v>6081.1404999999995</v>
+        <f>Forecast!B21*'Product Data'!C$2</f>
+        <v>24984.332499999997</v>
       </c>
       <c r="C21" s="8">
         <f>Forecast!C21*'Product Data'!$C$3</f>
@@ -7305,8 +7319,8 @@
         <v>57</v>
       </c>
       <c r="B22" s="8">
-        <f>ProductDataperState!G22*'Product Data'!C$2</f>
-        <v>5212.6983999999993</v>
+        <f>Forecast!B22*'Product Data'!C$2</f>
+        <v>22053.723999999998</v>
       </c>
       <c r="C22" s="8">
         <f>Forecast!C22*'Product Data'!$C$3</f>
@@ -7330,8 +7344,8 @@
         <v>58</v>
       </c>
       <c r="B23" s="8">
-        <f>ProductDataperState!G23*'Product Data'!C$2</f>
-        <v>1199.8616999999999</v>
+        <f>Forecast!B23*'Product Data'!C$2</f>
+        <v>4980.5000999999993</v>
       </c>
       <c r="C23" s="8">
         <f>Forecast!C23*'Product Data'!$C$3</f>
@@ -7355,8 +7369,8 @@
         <v>59</v>
       </c>
       <c r="B24" s="8">
-        <f>ProductDataperState!G24*'Product Data'!C$2</f>
-        <v>8664.9858999999997</v>
+        <f>Forecast!B24*'Product Data'!C$2</f>
+        <v>35816.843499999995</v>
       </c>
       <c r="C24" s="8">
         <f>Forecast!C24*'Product Data'!$C$3</f>
@@ -7380,8 +7394,8 @@
         <v>60</v>
       </c>
       <c r="B25" s="8">
-        <f>ProductDataperState!G25*'Product Data'!C$2</f>
-        <v>5009.1412999999993</v>
+        <f>Forecast!B25*'Product Data'!C$2</f>
+        <v>20475.389299999999</v>
       </c>
       <c r="C25" s="8">
         <f>Forecast!C25*'Product Data'!$C$3</f>
@@ -7405,8 +7419,8 @@
         <v>61</v>
       </c>
       <c r="B26" s="8">
-        <f>ProductDataperState!G26*'Product Data'!C$2</f>
-        <v>5269.9807999999994</v>
+        <f>Forecast!B26*'Product Data'!C$2</f>
+        <v>22111.006399999998</v>
       </c>
       <c r="C26" s="8">
         <f>Forecast!C26*'Product Data'!$C$3</f>
@@ -7430,8 +7444,8 @@
         <v>62</v>
       </c>
       <c r="B27" s="8">
-        <f>ProductDataperState!G27*'Product Data'!C$2</f>
-        <v>2584.8682999999996</v>
+        <f>Forecast!B27*'Product Data'!C$2</f>
+        <v>10489.8395</v>
       </c>
       <c r="C27" s="8">
         <f>Forecast!C27*'Product Data'!$C$3</f>
@@ -7455,8 +7469,8 @@
         <v>63</v>
       </c>
       <c r="B28" s="8">
-        <f>ProductDataperState!G28*'Product Data'!C$2</f>
-        <v>949.25119999999993</v>
+        <f>Forecast!B28*'Product Data'!C$2</f>
+        <v>4042.5007999999998</v>
       </c>
       <c r="C28" s="8">
         <f>Forecast!C28*'Product Data'!$C$3</f>
@@ -7480,8 +7494,8 @@
         <v>64</v>
       </c>
       <c r="B29" s="8">
-        <f>ProductDataperState!G29*'Product Data'!C$2</f>
-        <v>9451.5959999999995</v>
+        <f>Forecast!B29*'Product Data'!C$2</f>
+        <v>38665.619999999995</v>
       </c>
       <c r="C29" s="8">
         <f>Forecast!C29*'Product Data'!$C$3</f>
@@ -7505,8 +7519,8 @@
         <v>24</v>
       </c>
       <c r="B30" s="8">
-        <f>ProductDataperState!G30*'Product Data'!C$2</f>
-        <v>391.77069999999998</v>
+        <f>Forecast!B30*'Product Data'!C$2</f>
+        <v>2797.6315</v>
       </c>
       <c r="C30" s="8">
         <f>Forecast!C30*'Product Data'!$C$3</f>
@@ -7530,8 +7544,8 @@
         <v>65</v>
       </c>
       <c r="B31" s="8">
-        <f>ProductDataperState!G31*'Product Data'!C$2</f>
-        <v>1560.9453999999998</v>
+        <f>Forecast!B31*'Product Data'!C$2</f>
+        <v>7060.0557999999992</v>
       </c>
       <c r="C31" s="8">
         <f>Forecast!C31*'Product Data'!$C$3</f>
@@ -7555,8 +7569,8 @@
         <v>66</v>
       </c>
       <c r="B32" s="8">
-        <f>ProductDataperState!G32*'Product Data'!C$2</f>
-        <v>1222.3654999999999</v>
+        <f>Forecast!B32*'Product Data'!C$2</f>
+        <v>5003.0038999999997</v>
       </c>
       <c r="C32" s="8">
         <f>Forecast!C32*'Product Data'!$C$3</f>
@@ -7580,8 +7594,8 @@
         <v>67</v>
       </c>
       <c r="B33" s="8">
-        <f>ProductDataperState!G33*'Product Data'!C$2</f>
-        <v>8064.5435999999991</v>
+        <f>Forecast!B33*'Product Data'!C$2</f>
+        <v>33154.234799999998</v>
       </c>
       <c r="C33" s="8">
         <f>Forecast!C33*'Product Data'!$C$3</f>
@@ -7605,8 +7619,8 @@
         <v>68</v>
       </c>
       <c r="B34" s="8">
-        <f>ProductDataperState!G34*'Product Data'!C$2</f>
-        <v>1702.1055999999999</v>
+        <f>Forecast!B34*'Product Data'!C$2</f>
+        <v>7544.9103999999998</v>
       </c>
       <c r="C34" s="8">
         <f>Forecast!C34*'Product Data'!$C$3</f>
@@ -7630,8 +7644,8 @@
         <v>69</v>
       </c>
       <c r="B35" s="8">
-        <f>ProductDataperState!G35*'Product Data'!C$2</f>
-        <v>2805.8146999999999</v>
+        <f>Forecast!B35*'Product Data'!C$2</f>
+        <v>11398.1747</v>
       </c>
       <c r="C35" s="8">
         <f>Forecast!C35*'Product Data'!$C$3</f>
@@ -7655,8 +7669,8 @@
         <v>23</v>
       </c>
       <c r="B36" s="8">
-        <f>ProductDataperState!G36*'Product Data'!C$2</f>
-        <v>17253.254299999997</v>
+        <f>Forecast!B36*'Product Data'!C$2</f>
+        <v>69838.497499999998</v>
       </c>
       <c r="C36" s="8">
         <f>Forecast!C36*'Product Data'!$C$3</f>
@@ -7680,8 +7694,8 @@
         <v>70</v>
       </c>
       <c r="B37" s="8">
-        <f>ProductDataperState!G37*'Product Data'!C$2</f>
-        <v>10093.977199999999</v>
+        <f>Forecast!B37*'Product Data'!C$2</f>
+        <v>42057.556399999994</v>
       </c>
       <c r="C37" s="8">
         <f>Forecast!C37*'Product Data'!$C$3</f>
@@ -7705,8 +7719,8 @@
         <v>71</v>
       </c>
       <c r="B38" s="8">
-        <f>ProductDataperState!G38*'Product Data'!C$2</f>
-        <v>3467.6309999999999</v>
+        <f>Forecast!B38*'Product Data'!C$2</f>
+        <v>14465.851799999999</v>
       </c>
       <c r="C38" s="8">
         <f>Forecast!C38*'Product Data'!$C$3</f>
@@ -7730,8 +7744,8 @@
         <v>72</v>
       </c>
       <c r="B39" s="8">
-        <f>ProductDataperState!G39*'Product Data'!C$2</f>
-        <v>3420.5775999999996</v>
+        <f>Forecast!B39*'Product Data'!C$2</f>
+        <v>15106.187199999998</v>
       </c>
       <c r="C39" s="8">
         <f>Forecast!C39*'Product Data'!$C$3</f>
@@ -7756,8 +7770,8 @@
         <v>30</v>
       </c>
       <c r="B40" s="8">
-        <f>ProductDataperState!G40*'Product Data'!C$2</f>
-        <v>11195.6405</v>
+        <f>Forecast!B40*'Product Data'!C$2</f>
+        <v>46252.469299999997</v>
       </c>
       <c r="C40" s="8">
         <f>Forecast!C40*'Product Data'!$C$3</f>
@@ -7781,8 +7795,8 @@
         <v>73</v>
       </c>
       <c r="B41" s="8">
-        <f>ProductDataperState!G41*'Product Data'!C$2</f>
-        <v>817.29709999999989</v>
+        <f>Forecast!B41*'Product Data'!C$2</f>
+        <v>3910.5466999999999</v>
       </c>
       <c r="C41" s="8">
         <f>Forecast!C41*'Product Data'!$C$3</f>
@@ -7806,8 +7820,8 @@
         <v>74</v>
       </c>
       <c r="B42" s="8">
-        <f>ProductDataperState!G42*'Product Data'!C$2</f>
-        <v>4740.1185999999998</v>
+        <f>Forecast!B42*'Product Data'!C$2</f>
+        <v>19175.2834</v>
       </c>
       <c r="C42" s="8">
         <f>Forecast!C42*'Product Data'!$C$3</f>
@@ -7831,8 +7845,8 @@
         <v>75</v>
       </c>
       <c r="B43" s="8">
-        <f>ProductDataperState!G43*'Product Data'!C$2</f>
-        <v>530.88509999999997</v>
+        <f>Forecast!B43*'Product Data'!C$2</f>
+        <v>3280.4402999999998</v>
       </c>
       <c r="C43" s="8">
         <f>Forecast!C43*'Product Data'!$C$3</f>
@@ -7856,8 +7870,8 @@
         <v>29</v>
       </c>
       <c r="B44" s="8">
-        <f>ProductDataperState!G44*'Product Data'!C$2</f>
-        <v>6183.4304999999995</v>
+        <f>Forecast!B44*'Product Data'!C$2</f>
+        <v>25430.316899999998</v>
       </c>
       <c r="C44" s="8">
         <f>Forecast!C44*'Product Data'!$C$3</f>
@@ -7881,8 +7895,8 @@
         <v>26</v>
       </c>
       <c r="B45" s="8">
-        <f>ProductDataperState!G45*'Product Data'!C$2</f>
-        <v>26705.873199999998</v>
+        <f>Forecast!B45*'Product Data'!C$2</f>
+        <v>108848.8348</v>
       </c>
       <c r="C45" s="8">
         <f>Forecast!C45*'Product Data'!$C$3</f>
@@ -7906,8 +7920,8 @@
         <v>31</v>
       </c>
       <c r="B46" s="8">
-        <f>ProductDataperState!G46*'Product Data'!C$2</f>
-        <v>2916.2878999999998</v>
+        <f>Forecast!B46*'Product Data'!C$2</f>
+        <v>12196.036699999999</v>
       </c>
       <c r="C46" s="8">
         <f>Forecast!C46*'Product Data'!$C$3</f>
@@ -7931,8 +7945,8 @@
         <v>76</v>
       </c>
       <c r="B47" s="8">
-        <f>ProductDataperState!G47*'Product Data'!C$2</f>
-        <v>7386.3608999999997</v>
+        <f>Forecast!B47*'Product Data'!C$2</f>
+        <v>31101.274499999996</v>
       </c>
       <c r="C47" s="8">
         <f>Forecast!C47*'Product Data'!$C$3</f>
@@ -7956,8 +7970,8 @@
         <v>77</v>
       </c>
       <c r="B48" s="8">
-        <f>ProductDataperState!G48*'Product Data'!C$2</f>
-        <v>248.56469999999999</v>
+        <f>Forecast!B48*'Product Data'!C$2</f>
+        <v>2310.7311</v>
       </c>
       <c r="C48" s="8">
         <f>Forecast!C48*'Product Data'!$C$3</f>
@@ -7981,8 +7995,8 @@
         <v>32</v>
       </c>
       <c r="B49" s="8">
-        <f>ProductDataperState!G49*'Product Data'!C$2</f>
-        <v>6571.1095999999998</v>
+        <f>Forecast!B49*'Product Data'!C$2</f>
+        <v>27880.162399999997</v>
       </c>
       <c r="C49" s="8">
         <f>Forecast!C49*'Product Data'!$C$3</f>
@@ -8007,8 +8021,8 @@
         <v>78</v>
       </c>
       <c r="B50" s="8">
-        <f>ProductDataperState!G50*'Product Data'!C$2</f>
-        <v>4939.5841</v>
+        <f>Forecast!B50*'Product Data'!C$2</f>
+        <v>21093.220899999997</v>
       </c>
       <c r="C50" s="8">
         <f>Forecast!C50*'Product Data'!$C$3</f>
@@ -8032,8 +8046,8 @@
         <v>79</v>
       </c>
       <c r="B51" s="8">
-        <f>ProductDataperState!G51*'Product Data'!C$2</f>
-        <v>1504.6858999999999</v>
+        <f>Forecast!B51*'Product Data'!C$2</f>
+        <v>6316.4074999999993</v>
       </c>
       <c r="C51" s="8">
         <f>Forecast!C51*'Product Data'!$C$3</f>
@@ -8057,8 +8071,8 @@
         <v>80</v>
       </c>
       <c r="B52" s="8">
-        <f>ProductDataperState!G52*'Product Data'!C$2</f>
-        <v>366.19819999999999</v>
+        <f>Forecast!B52*'Product Data'!C$2</f>
+        <v>2084.6702</v>
       </c>
       <c r="C52" s="8">
         <f>Forecast!C52*'Product Data'!$C$3</f>
@@ -8083,6 +8097,1997 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1BAE6A-2363-4B17-8357-E84D9D57E6E7}">
+  <dimension ref="A1:L52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D2">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="E2">
+        <v>0.1754</v>
+      </c>
+      <c r="F2">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="G2">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H2">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I2">
+        <v>0.2631</v>
+      </c>
+      <c r="J2">
+        <v>0.3105</v>
+      </c>
+      <c r="K2">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="L2">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3">
+        <v>0.2036</v>
+      </c>
+      <c r="D3">
+        <v>0.1754</v>
+      </c>
+      <c r="E3">
+        <v>0.3105</v>
+      </c>
+      <c r="F3">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G3">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="H3">
+        <v>0.2631</v>
+      </c>
+      <c r="I3">
+        <v>0.2631</v>
+      </c>
+      <c r="J3">
+        <v>0.3105</v>
+      </c>
+      <c r="K3">
+        <v>0.1754</v>
+      </c>
+      <c r="L3">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4">
+        <v>0.2036</v>
+      </c>
+      <c r="D4">
+        <v>0.1754</v>
+      </c>
+      <c r="E4">
+        <v>0.2631</v>
+      </c>
+      <c r="F4">
+        <v>0.3105</v>
+      </c>
+      <c r="G4">
+        <v>5.67E-2</v>
+      </c>
+      <c r="H4">
+        <v>0.2631</v>
+      </c>
+      <c r="I4">
+        <v>0.2036</v>
+      </c>
+      <c r="J4">
+        <v>0.2631</v>
+      </c>
+      <c r="K4">
+        <v>5.67E-2</v>
+      </c>
+      <c r="L4">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.3105</v>
+      </c>
+      <c r="E5">
+        <v>0.1754</v>
+      </c>
+      <c r="F5">
+        <v>0.2631</v>
+      </c>
+      <c r="G5">
+        <v>0.2036</v>
+      </c>
+      <c r="H5">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I5">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="J5">
+        <v>0.2631</v>
+      </c>
+      <c r="K5">
+        <v>0.1754</v>
+      </c>
+      <c r="L5">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.3105</v>
+      </c>
+      <c r="E6">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.2036</v>
+      </c>
+      <c r="G6">
+        <v>0.2631</v>
+      </c>
+      <c r="H6">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I6">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="J6">
+        <v>0.3105</v>
+      </c>
+      <c r="K6">
+        <v>0.2036</v>
+      </c>
+      <c r="L6">
+        <v>0.2631</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7">
+        <v>0.3105</v>
+      </c>
+      <c r="D7">
+        <v>0.2036</v>
+      </c>
+      <c r="E7">
+        <v>0.2036</v>
+      </c>
+      <c r="F7">
+        <v>0.2631</v>
+      </c>
+      <c r="G7">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I7">
+        <v>5.67E-2</v>
+      </c>
+      <c r="J7">
+        <v>0.1754</v>
+      </c>
+      <c r="K7">
+        <v>5.67E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.2036</v>
+      </c>
+      <c r="E8">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F8">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G8">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H8">
+        <v>5.67E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J8">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K8">
+        <v>0.3105</v>
+      </c>
+      <c r="L8">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.2036</v>
+      </c>
+      <c r="E9">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F9">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G9">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H9">
+        <v>5.67E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J9">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K9">
+        <v>0.3105</v>
+      </c>
+      <c r="L9">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10">
+        <v>0.2036</v>
+      </c>
+      <c r="D10">
+        <v>0.2036</v>
+      </c>
+      <c r="E10">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F10">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.2036</v>
+      </c>
+      <c r="H10">
+        <v>0.2036</v>
+      </c>
+      <c r="I10">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J10">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K10">
+        <v>0.2631</v>
+      </c>
+      <c r="L10">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11">
+        <v>0.2036</v>
+      </c>
+      <c r="D11">
+        <v>0.1754</v>
+      </c>
+      <c r="E11">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F11">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.2036</v>
+      </c>
+      <c r="H11">
+        <v>0.2036</v>
+      </c>
+      <c r="I11">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J11">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K11">
+        <v>0.2036</v>
+      </c>
+      <c r="L11">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D12">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F12">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G12">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H12">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I12">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J12">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="L12">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13">
+        <v>0.2036</v>
+      </c>
+      <c r="D13">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.2631</v>
+      </c>
+      <c r="F13">
+        <v>0.3105</v>
+      </c>
+      <c r="G13">
+        <v>0.1754</v>
+      </c>
+      <c r="H13">
+        <v>0.2631</v>
+      </c>
+      <c r="I13">
+        <v>0.1754</v>
+      </c>
+      <c r="J13">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="K13">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L13">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D14">
+        <v>0.3105</v>
+      </c>
+      <c r="E14">
+        <v>0.2036</v>
+      </c>
+      <c r="F14">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H14">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I14">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="J14">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="K14">
+        <v>0.1754</v>
+      </c>
+      <c r="L14">
+        <v>0.2631</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15">
+        <v>0.2036</v>
+      </c>
+      <c r="D15">
+        <v>5.67E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.3105</v>
+      </c>
+      <c r="F15">
+        <v>0.3105</v>
+      </c>
+      <c r="G15">
+        <v>0.2036</v>
+      </c>
+      <c r="H15">
+        <v>0.1754</v>
+      </c>
+      <c r="I15">
+        <v>0.2036</v>
+      </c>
+      <c r="J15">
+        <v>0.2036</v>
+      </c>
+      <c r="K15">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L15">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16">
+        <v>0.1754</v>
+      </c>
+      <c r="D16">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.3105</v>
+      </c>
+      <c r="F16">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G16">
+        <v>0.2631</v>
+      </c>
+      <c r="H16">
+        <v>0.1754</v>
+      </c>
+      <c r="I16">
+        <v>0.2631</v>
+      </c>
+      <c r="J16">
+        <v>5.67E-2</v>
+      </c>
+      <c r="K16">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L16">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17">
+        <v>0.2631</v>
+      </c>
+      <c r="D17">
+        <v>0.1754</v>
+      </c>
+      <c r="E17">
+        <v>0.2631</v>
+      </c>
+      <c r="F17">
+        <v>0.3105</v>
+      </c>
+      <c r="G17">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="H17">
+        <v>0.3105</v>
+      </c>
+      <c r="I17">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="J17">
+        <v>0.1754</v>
+      </c>
+      <c r="K17">
+        <v>5.67E-2</v>
+      </c>
+      <c r="L17">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18">
+        <v>0.1754</v>
+      </c>
+      <c r="D18">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.3105</v>
+      </c>
+      <c r="F18">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G18">
+        <v>0.1754</v>
+      </c>
+      <c r="H18">
+        <v>0.1754</v>
+      </c>
+      <c r="I18">
+        <v>0.2631</v>
+      </c>
+      <c r="J18">
+        <v>0.2631</v>
+      </c>
+      <c r="K18">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L18">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19">
+        <v>0.2631</v>
+      </c>
+      <c r="D19">
+        <v>0.2036</v>
+      </c>
+      <c r="E19">
+        <v>0.3105</v>
+      </c>
+      <c r="F19">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G19">
+        <v>5.67E-2</v>
+      </c>
+      <c r="H19">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I19">
+        <v>0.2631</v>
+      </c>
+      <c r="J19">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K19">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L19">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.2036</v>
+      </c>
+      <c r="E20">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F20">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H20">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="I20">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J20">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K20">
+        <v>0.3105</v>
+      </c>
+      <c r="L20">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21">
+        <v>5.67E-2</v>
+      </c>
+      <c r="D21">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="E21">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F21">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G21">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H21">
+        <v>5.67E-2</v>
+      </c>
+      <c r="I21">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J21">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K21">
+        <v>0.3105</v>
+      </c>
+      <c r="L21">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22">
+        <v>0.1754</v>
+      </c>
+      <c r="D22">
+        <v>0.2036</v>
+      </c>
+      <c r="E22">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F22">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G22">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H22">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="I22">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J22">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K22">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="L22">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23">
+        <v>0.1754</v>
+      </c>
+      <c r="D23">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="E23">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F23">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G23">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H23">
+        <v>0.2631</v>
+      </c>
+      <c r="I23">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J23">
+        <v>0.2631</v>
+      </c>
+      <c r="K23">
+        <v>0.1754</v>
+      </c>
+      <c r="L23">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24">
+        <v>0.2036</v>
+      </c>
+      <c r="D24">
+        <v>0.1754</v>
+      </c>
+      <c r="E24">
+        <v>0.3105</v>
+      </c>
+      <c r="F24">
+        <v>0.2631</v>
+      </c>
+      <c r="G24">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H24">
+        <v>0.2631</v>
+      </c>
+      <c r="I24">
+        <v>0.2631</v>
+      </c>
+      <c r="J24">
+        <v>0.1754</v>
+      </c>
+      <c r="K24">
+        <v>0.1754</v>
+      </c>
+      <c r="L24">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25">
+        <v>0.2036</v>
+      </c>
+      <c r="D25">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="E25">
+        <v>0.3105</v>
+      </c>
+      <c r="F25">
+        <v>0.3105</v>
+      </c>
+      <c r="G25">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="H25">
+        <v>0.2036</v>
+      </c>
+      <c r="I25">
+        <v>0.1754</v>
+      </c>
+      <c r="J25">
+        <v>0.2036</v>
+      </c>
+      <c r="K25">
+        <v>5.67E-2</v>
+      </c>
+      <c r="L25">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26">
+        <v>0.2036</v>
+      </c>
+      <c r="D26">
+        <v>0.2036</v>
+      </c>
+      <c r="E26">
+        <v>0.3105</v>
+      </c>
+      <c r="F26">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G26">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="H26">
+        <v>0.2631</v>
+      </c>
+      <c r="I26">
+        <v>0.2036</v>
+      </c>
+      <c r="J26">
+        <v>0.3105</v>
+      </c>
+      <c r="K26">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L26">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D27">
+        <v>0.2036</v>
+      </c>
+      <c r="E27">
+        <v>0.1754</v>
+      </c>
+      <c r="F27">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="G27">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H27">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I27">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="J27">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="K27">
+        <v>0.1754</v>
+      </c>
+      <c r="L27">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28">
+        <v>0.1754</v>
+      </c>
+      <c r="D28">
+        <v>0.1754</v>
+      </c>
+      <c r="E28">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F28">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G28">
+        <v>0.1754</v>
+      </c>
+      <c r="H28">
+        <v>0.1754</v>
+      </c>
+      <c r="I28">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J28">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K28">
+        <v>0.2036</v>
+      </c>
+      <c r="L28">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29">
+        <v>0.2631</v>
+      </c>
+      <c r="D29">
+        <v>0.2036</v>
+      </c>
+      <c r="E29">
+        <v>0.2631</v>
+      </c>
+      <c r="F29">
+        <v>0.2631</v>
+      </c>
+      <c r="G29">
+        <v>0.3105</v>
+      </c>
+      <c r="H29">
+        <v>0.3105</v>
+      </c>
+      <c r="I29">
+        <v>0.2036</v>
+      </c>
+      <c r="J29">
+        <v>5.67E-2</v>
+      </c>
+      <c r="K29">
+        <v>0.1754</v>
+      </c>
+      <c r="L29">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30">
+        <v>0.2631</v>
+      </c>
+      <c r="D30">
+        <v>0.1754</v>
+      </c>
+      <c r="E30">
+        <v>0.2631</v>
+      </c>
+      <c r="F30">
+        <v>0.2631</v>
+      </c>
+      <c r="G30">
+        <v>0.1754</v>
+      </c>
+      <c r="H30">
+        <v>0.3105</v>
+      </c>
+      <c r="I30">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="J30">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="K30">
+        <v>5.67E-2</v>
+      </c>
+      <c r="L30">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="D31">
+        <v>0.2036</v>
+      </c>
+      <c r="E31">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F31">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G31">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H31">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="I31">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J31">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K31">
+        <v>0.3105</v>
+      </c>
+      <c r="L31">
+        <v>0.2631</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="D32">
+        <v>0.2036</v>
+      </c>
+      <c r="E32">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F32">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G32">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H32">
+        <v>5.67E-2</v>
+      </c>
+      <c r="I32">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J32">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K32">
+        <v>0.3105</v>
+      </c>
+      <c r="L32">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33">
+        <v>0.3105</v>
+      </c>
+      <c r="D33">
+        <v>0.2631</v>
+      </c>
+      <c r="E33">
+        <v>0.2036</v>
+      </c>
+      <c r="F33">
+        <v>0.2631</v>
+      </c>
+      <c r="G33">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="H33">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I33">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="J33">
+        <v>0.2631</v>
+      </c>
+      <c r="K33">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L33">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D34">
+        <v>0.3105</v>
+      </c>
+      <c r="E34">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="F34">
+        <v>0.2036</v>
+      </c>
+      <c r="G34">
+        <v>0.2036</v>
+      </c>
+      <c r="H34">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I34">
+        <v>5.67E-2</v>
+      </c>
+      <c r="J34">
+        <v>0.2036</v>
+      </c>
+      <c r="K34">
+        <v>0.1754</v>
+      </c>
+      <c r="L34">
+        <v>0.3105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="D35">
+        <v>0.2036</v>
+      </c>
+      <c r="E35">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F35">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G35">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H35">
+        <v>5.67E-2</v>
+      </c>
+      <c r="I35">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J35">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K35">
+        <v>0.3105</v>
+      </c>
+      <c r="L35">
+        <v>0.2631</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36">
+        <v>0.1754</v>
+      </c>
+      <c r="D36">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="E36">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F36">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G36">
+        <v>0.2631</v>
+      </c>
+      <c r="H36">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="I36">
+        <v>0.2631</v>
+      </c>
+      <c r="J36">
+        <v>0.2036</v>
+      </c>
+      <c r="K36">
+        <v>0.1754</v>
+      </c>
+      <c r="L36">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37">
+        <v>0.2631</v>
+      </c>
+      <c r="D37">
+        <v>0.2036</v>
+      </c>
+      <c r="E37">
+        <v>0.2631</v>
+      </c>
+      <c r="F37">
+        <v>0.3105</v>
+      </c>
+      <c r="G37">
+        <v>5.67E-2</v>
+      </c>
+      <c r="H37">
+        <v>0.3105</v>
+      </c>
+      <c r="I37">
+        <v>0.1754</v>
+      </c>
+      <c r="J37">
+        <v>0.2631</v>
+      </c>
+      <c r="K37">
+        <v>5.67E-2</v>
+      </c>
+      <c r="L37">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D38">
+        <v>0.3105</v>
+      </c>
+      <c r="E38">
+        <v>0.2036</v>
+      </c>
+      <c r="F38">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="G38">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H38">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I38">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="J38">
+        <v>0.1754</v>
+      </c>
+      <c r="K38">
+        <v>0.2631</v>
+      </c>
+      <c r="L38">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="D39">
+        <v>0.1754</v>
+      </c>
+      <c r="E39">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F39">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G39">
+        <v>0.2631</v>
+      </c>
+      <c r="H39">
+        <v>0.2631</v>
+      </c>
+      <c r="I39">
+        <v>0.2036</v>
+      </c>
+      <c r="J39">
+        <v>0.2631</v>
+      </c>
+      <c r="K39">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L39">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="D40">
+        <v>0.2036</v>
+      </c>
+      <c r="E40">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F40">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G40">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H40">
+        <v>5.67E-2</v>
+      </c>
+      <c r="I40">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J40">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K40">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="L40">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41">
+        <v>0.1754</v>
+      </c>
+      <c r="D41">
+        <v>0.2036</v>
+      </c>
+      <c r="E41">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F41">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G41">
+        <v>0.1754</v>
+      </c>
+      <c r="H41">
+        <v>0.2036</v>
+      </c>
+      <c r="I41">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J41">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K41">
+        <v>0.1754</v>
+      </c>
+      <c r="L41">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42">
+        <v>0.2631</v>
+      </c>
+      <c r="D42">
+        <v>0.1754</v>
+      </c>
+      <c r="E42">
+        <v>0.2631</v>
+      </c>
+      <c r="F42">
+        <v>0.2631</v>
+      </c>
+      <c r="G42">
+        <v>0.2036</v>
+      </c>
+      <c r="H42">
+        <v>0.2631</v>
+      </c>
+      <c r="I42">
+        <v>0.1754</v>
+      </c>
+      <c r="J42">
+        <v>5.67E-2</v>
+      </c>
+      <c r="K42">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L42">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43">
+        <v>0.2036</v>
+      </c>
+      <c r="D43">
+        <v>0.1754</v>
+      </c>
+      <c r="E43">
+        <v>0.3105</v>
+      </c>
+      <c r="F43">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G43">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="H43">
+        <v>0.1754</v>
+      </c>
+      <c r="I43">
+        <v>0.2631</v>
+      </c>
+      <c r="J43">
+        <v>0.2036</v>
+      </c>
+      <c r="K43">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L43">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44">
+        <v>0.2631</v>
+      </c>
+      <c r="D44">
+        <v>0.2036</v>
+      </c>
+      <c r="E44">
+        <v>0.2631</v>
+      </c>
+      <c r="F44">
+        <v>0.3105</v>
+      </c>
+      <c r="G44">
+        <v>5.67E-2</v>
+      </c>
+      <c r="H44">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I44">
+        <v>0.1754</v>
+      </c>
+      <c r="J44">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K44">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L44">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D45">
+        <v>0.2631</v>
+      </c>
+      <c r="E45">
+        <v>0.1754</v>
+      </c>
+      <c r="F45">
+        <v>0.2036</v>
+      </c>
+      <c r="G45">
+        <v>0.3105</v>
+      </c>
+      <c r="H45">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I45">
+        <v>5.67E-2</v>
+      </c>
+      <c r="J45">
+        <v>0.1754</v>
+      </c>
+      <c r="K45">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L45">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="D46">
+        <v>0.1754</v>
+      </c>
+      <c r="E46">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F46">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G46">
+        <v>0.2631</v>
+      </c>
+      <c r="H46">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="I46">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J46">
+        <v>0.3105</v>
+      </c>
+      <c r="K46">
+        <v>0.1754</v>
+      </c>
+      <c r="L46">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="D47">
+        <v>0.2036</v>
+      </c>
+      <c r="E47">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F47">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G47">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H47">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="I47">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J47">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K47">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="L47">
+        <v>0.3105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="D48">
+        <v>0.3105</v>
+      </c>
+      <c r="E48">
+        <v>0.2036</v>
+      </c>
+      <c r="F48">
+        <v>5.67E-2</v>
+      </c>
+      <c r="G48">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H48">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I48">
+        <v>0.1754</v>
+      </c>
+      <c r="J48">
+        <v>0.1754</v>
+      </c>
+      <c r="K48">
+        <v>0.3105</v>
+      </c>
+      <c r="L48">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49">
+        <v>0.2036</v>
+      </c>
+      <c r="D49">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="E49">
+        <v>0.3105</v>
+      </c>
+      <c r="F49">
+        <v>0.3105</v>
+      </c>
+      <c r="G49">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H49">
+        <v>0.2631</v>
+      </c>
+      <c r="I49">
+        <v>0.2036</v>
+      </c>
+      <c r="J49">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="K49">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L49">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50">
+        <v>0.1754</v>
+      </c>
+      <c r="D50">
+        <v>0.1754</v>
+      </c>
+      <c r="E50">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F50">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G50">
+        <v>0.2631</v>
+      </c>
+      <c r="H50">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="I50">
+        <v>0.3105</v>
+      </c>
+      <c r="J50">
+        <v>0.1754</v>
+      </c>
+      <c r="K50">
+        <v>0.1754</v>
+      </c>
+      <c r="L50">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51">
+        <v>0.3105</v>
+      </c>
+      <c r="D51">
+        <v>0.2036</v>
+      </c>
+      <c r="E51">
+        <v>0.2036</v>
+      </c>
+      <c r="F51">
+        <v>0.2036</v>
+      </c>
+      <c r="G51">
+        <v>0.2036</v>
+      </c>
+      <c r="H51">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="I51">
+        <v>5.67E-2</v>
+      </c>
+      <c r="J51">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="K51">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L51">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52">
+        <v>5.67E-2</v>
+      </c>
+      <c r="D52">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="E52">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="F52">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="G52">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="H52">
+        <v>5.67E-2</v>
+      </c>
+      <c r="I52">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="J52">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="K52">
+        <v>0.3105</v>
+      </c>
+      <c r="L52">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -8516,7 +10521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>